<commit_message>
Adds and updates spreadsheets for my Medium blog
</commit_message>
<xml_diff>
--- a/Blog/CookieCutterEstimates.xlsx
+++ b/Blog/CookieCutterEstimates.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiberius/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiberius/Documents/Codigo/FilipeAlberoPomar/Blog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD62743-A6DF-CE4D-A315-D7877F751E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB819B2-1FC5-C746-82DE-781780A8F924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{9B2DFC66-3B81-9246-BCCA-9F8999403033}"/>
   </bookViews>
@@ -654,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F616CA93-097B-AF4A-945A-813C6AED0C91}">
-  <dimension ref="B1:G20"/>
+  <dimension ref="B1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,13 +669,13 @@
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="2:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="15" t="s">
@@ -684,11 +684,8 @@
       <c r="E2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="16" t="s">
         <v>2</v>
       </c>
@@ -702,7 +699,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="17"/>
       <c r="C4" s="1" t="s">
         <v>1</v>
@@ -714,13 +711,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="18"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="16" t="s">
         <v>3</v>
       </c>
@@ -734,7 +731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="17"/>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -746,7 +743,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="17"/>
       <c r="C8" s="1" t="s">
         <v>6</v>
@@ -758,13 +755,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="18"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="16" t="s">
         <v>7</v>
       </c>
@@ -778,7 +775,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="17"/>
       <c r="C11" s="1" t="s">
         <v>9</v>
@@ -790,7 +787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="17"/>
       <c r="C12" s="1" t="s">
         <v>10</v>
@@ -802,13 +799,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="18"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="16" t="s">
         <v>11</v>
       </c>
@@ -822,7 +819,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C15" s="1" t="s">
         <v>13</v>
       </c>
@@ -833,14 +830,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
@@ -854,7 +851,7 @@
       </c>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C19" s="13" t="s">
         <v>15</v>
       </c>
@@ -868,7 +865,7 @@
       </c>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C20" s="14" t="s">
         <v>16</v>
       </c>
@@ -879,6 +876,11 @@
       <c r="E20" s="11">
         <f>E18/22</f>
         <v>4.0454545454545459</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>